<commit_message>
Finished first version of website
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2023-02-04</t>
+          <t>2023-02-06</t>
         </is>
       </c>
     </row>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -497,24 +497,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>5 Musketeers</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Loose Gooses</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>5 Musketeers</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Angus</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -523,102 +523,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>5 Musketeers</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Wet Willies</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Loose Gooses</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Kimmy</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Wet Willies</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5 Musketeers</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Rudy</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Loose Gooses</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Wet Willies</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Clarrie</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>5 Musketeers</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Loose Gooses</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Kimmy</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>